<commit_message>
removed extra lines in sample data file for unit tests
</commit_message>
<xml_diff>
--- a/tests/sample_data/100.xlsx
+++ b/tests/sample_data/100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celia.maiorano/Python_Repositories/MoBI-Motion-Tracking-Development-branches/data_loader/mobi-motion-tracking/tests/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192668A4-21B1-AE4A-9E20-308859B9AEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03090D1B-55BE-C04F-8663-E6D45E1C5988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -688,7 +688,7 @@
   <dimension ref="A1:BV1752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4580,746 +4580,6 @@
         <v>-3.6530300000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>221</v>
-      </c>
-      <c r="B26">
-        <v>1.57192</v>
-      </c>
-      <c r="C26">
-        <v>-11.9323</v>
-      </c>
-      <c r="D26">
-        <v>1.5428299999999999</v>
-      </c>
-      <c r="E26">
-        <v>0.42374200000000001</v>
-      </c>
-      <c r="F26">
-        <v>-3.0090499999999998</v>
-      </c>
-      <c r="G26">
-        <v>-3.6140500000000002</v>
-      </c>
-      <c r="H26">
-        <v>-0.41601700000000003</v>
-      </c>
-      <c r="I26">
-        <v>5.2797000000000001</v>
-      </c>
-      <c r="J26">
-        <v>-3.3879999999999999</v>
-      </c>
-      <c r="K26">
-        <v>-1.21377</v>
-      </c>
-      <c r="L26">
-        <v>15.512</v>
-      </c>
-      <c r="M26">
-        <v>-5.8332699999999997</v>
-      </c>
-      <c r="N26">
-        <v>-7.4063199999999996E-2</v>
-      </c>
-      <c r="O26">
-        <v>38.6965</v>
-      </c>
-      <c r="P26">
-        <v>-5.8971400000000003</v>
-      </c>
-      <c r="Q26">
-        <v>0.73716599999999999</v>
-      </c>
-      <c r="R26">
-        <v>51.711500000000001</v>
-      </c>
-      <c r="S26">
-        <v>-2.1004</v>
-      </c>
-      <c r="T26">
-        <v>-2.0961099999999999</v>
-      </c>
-      <c r="U26">
-        <v>37.8369</v>
-      </c>
-      <c r="V26">
-        <v>2.3391500000000001</v>
-      </c>
-      <c r="W26">
-        <v>-16.361999999999998</v>
-      </c>
-      <c r="X26">
-        <v>38.469000000000001</v>
-      </c>
-      <c r="Y26">
-        <v>-2.2290000000000001</v>
-      </c>
-      <c r="Z26">
-        <v>-24.355</v>
-      </c>
-      <c r="AA26">
-        <v>11.5778</v>
-      </c>
-      <c r="AB26">
-        <v>-9.8761899999999994</v>
-      </c>
-      <c r="AC26">
-        <v>-26.7836</v>
-      </c>
-      <c r="AD26">
-        <v>-11.911300000000001</v>
-      </c>
-      <c r="AE26">
-        <v>-15.4194</v>
-      </c>
-      <c r="AF26">
-        <v>2.5795300000000001</v>
-      </c>
-      <c r="AG26">
-        <v>37.606499999999997</v>
-      </c>
-      <c r="AH26">
-        <v>2.1299700000000001</v>
-      </c>
-      <c r="AI26">
-        <v>16.390699999999999</v>
-      </c>
-      <c r="AJ26">
-        <v>37.239699999999999</v>
-      </c>
-      <c r="AK26">
-        <v>-3.6856599999999999</v>
-      </c>
-      <c r="AL26">
-        <v>20.3491</v>
-      </c>
-      <c r="AM26">
-        <v>11.4697</v>
-      </c>
-      <c r="AN26">
-        <v>9.1882800000000007</v>
-      </c>
-      <c r="AO26">
-        <v>13.3392</v>
-      </c>
-      <c r="AP26">
-        <v>34.648099999999999</v>
-      </c>
-      <c r="AQ26">
-        <v>10.598100000000001</v>
-      </c>
-      <c r="AR26">
-        <v>-8.5826600000000006</v>
-      </c>
-      <c r="AS26">
-        <v>-8.8508999999999993</v>
-      </c>
-      <c r="AT26">
-        <v>1.0749200000000001</v>
-      </c>
-      <c r="AU26">
-        <v>-8.7301800000000007</v>
-      </c>
-      <c r="AV26">
-        <v>-50.122300000000003</v>
-      </c>
-      <c r="AW26">
-        <v>10.9771</v>
-      </c>
-      <c r="AX26">
-        <v>-9.4173500000000008</v>
-      </c>
-      <c r="AY26">
-        <v>-90.185599999999994</v>
-      </c>
-      <c r="AZ26">
-        <v>-0.45941500000000002</v>
-      </c>
-      <c r="BA26">
-        <v>10.8086</v>
-      </c>
-      <c r="BB26">
-        <v>-6.86212</v>
-      </c>
-      <c r="BC26">
-        <v>0.19825400000000001</v>
-      </c>
-      <c r="BD26">
-        <v>10.8088</v>
-      </c>
-      <c r="BE26">
-        <v>-49.256999999999998</v>
-      </c>
-      <c r="BF26">
-        <v>-1.8266</v>
-      </c>
-      <c r="BG26">
-        <v>7.5135100000000001</v>
-      </c>
-      <c r="BH26">
-        <v>-90.762699999999995</v>
-      </c>
-      <c r="BI26">
-        <v>-3.48631</v>
-      </c>
-    </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>222</v>
-      </c>
-      <c r="B27">
-        <v>1.54037</v>
-      </c>
-      <c r="C27">
-        <v>-11.915800000000001</v>
-      </c>
-      <c r="D27">
-        <v>1.46262</v>
-      </c>
-      <c r="E27">
-        <v>0.33643499999999998</v>
-      </c>
-      <c r="F27">
-        <v>-2.9996800000000001</v>
-      </c>
-      <c r="G27">
-        <v>-3.6937799999999998</v>
-      </c>
-      <c r="H27">
-        <v>-0.51635299999999995</v>
-      </c>
-      <c r="I27">
-        <v>5.2877900000000002</v>
-      </c>
-      <c r="J27">
-        <v>-3.4691999999999998</v>
-      </c>
-      <c r="K27">
-        <v>-1.34616</v>
-      </c>
-      <c r="L27">
-        <v>15.521100000000001</v>
-      </c>
-      <c r="M27">
-        <v>-5.8997700000000002</v>
-      </c>
-      <c r="N27">
-        <v>-0.180316</v>
-      </c>
-      <c r="O27">
-        <v>38.7042</v>
-      </c>
-      <c r="P27">
-        <v>-5.8208900000000003</v>
-      </c>
-      <c r="Q27">
-        <v>0.68687399999999998</v>
-      </c>
-      <c r="R27">
-        <v>51.692599999999999</v>
-      </c>
-      <c r="S27">
-        <v>-1.94617</v>
-      </c>
-      <c r="T27">
-        <v>-2.11449</v>
-      </c>
-      <c r="U27">
-        <v>37.791600000000003</v>
-      </c>
-      <c r="V27">
-        <v>2.4308100000000001</v>
-      </c>
-      <c r="W27">
-        <v>-16.427900000000001</v>
-      </c>
-      <c r="X27">
-        <v>38.471600000000002</v>
-      </c>
-      <c r="Y27">
-        <v>-1.97888</v>
-      </c>
-      <c r="Z27">
-        <v>-23.924800000000001</v>
-      </c>
-      <c r="AA27">
-        <v>11.621499999999999</v>
-      </c>
-      <c r="AB27">
-        <v>-10.2475</v>
-      </c>
-      <c r="AC27">
-        <v>-25.979800000000001</v>
-      </c>
-      <c r="AD27">
-        <v>-11.884</v>
-      </c>
-      <c r="AE27">
-        <v>-15.8718</v>
-      </c>
-      <c r="AF27">
-        <v>2.5583499999999999</v>
-      </c>
-      <c r="AG27">
-        <v>37.557499999999997</v>
-      </c>
-      <c r="AH27">
-        <v>2.16967</v>
-      </c>
-      <c r="AI27">
-        <v>16.307700000000001</v>
-      </c>
-      <c r="AJ27">
-        <v>37.277000000000001</v>
-      </c>
-      <c r="AK27">
-        <v>-3.7953000000000001</v>
-      </c>
-      <c r="AL27">
-        <v>21.044699999999999</v>
-      </c>
-      <c r="AM27">
-        <v>11.699400000000001</v>
-      </c>
-      <c r="AN27">
-        <v>9.1988800000000008</v>
-      </c>
-      <c r="AO27">
-        <v>13.1858</v>
-      </c>
-      <c r="AP27">
-        <v>34.579599999999999</v>
-      </c>
-      <c r="AQ27">
-        <v>10.9588</v>
-      </c>
-      <c r="AR27">
-        <v>-8.6230100000000007</v>
-      </c>
-      <c r="AS27">
-        <v>-8.8529599999999995</v>
-      </c>
-      <c r="AT27">
-        <v>1.0702700000000001</v>
-      </c>
-      <c r="AU27">
-        <v>-8.8107900000000008</v>
-      </c>
-      <c r="AV27">
-        <v>-50.159100000000002</v>
-      </c>
-      <c r="AW27">
-        <v>10.826000000000001</v>
-      </c>
-      <c r="AX27">
-        <v>-9.4135500000000008</v>
-      </c>
-      <c r="AY27">
-        <v>-90.377899999999997</v>
-      </c>
-      <c r="AZ27">
-        <v>-5.5888300000000002E-2</v>
-      </c>
-      <c r="BA27">
-        <v>10.757300000000001</v>
-      </c>
-      <c r="BB27">
-        <v>-6.8305499999999997</v>
-      </c>
-      <c r="BC27">
-        <v>4.1818599999999997E-2</v>
-      </c>
-      <c r="BD27">
-        <v>10.936999999999999</v>
-      </c>
-      <c r="BE27">
-        <v>-49.235900000000001</v>
-      </c>
-      <c r="BF27">
-        <v>-1.74319</v>
-      </c>
-      <c r="BG27">
-        <v>7.7054900000000002</v>
-      </c>
-      <c r="BH27">
-        <v>-90.748400000000004</v>
-      </c>
-      <c r="BI27">
-        <v>-3.35541</v>
-      </c>
-    </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>223</v>
-      </c>
-      <c r="B28">
-        <v>1.5099800000000001</v>
-      </c>
-      <c r="C28">
-        <v>-11.8932</v>
-      </c>
-      <c r="D28">
-        <v>1.3859399999999999</v>
-      </c>
-      <c r="E28">
-        <v>0.217476</v>
-      </c>
-      <c r="F28">
-        <v>-2.9908299999999999</v>
-      </c>
-      <c r="G28">
-        <v>-3.7728999999999999</v>
-      </c>
-      <c r="H28">
-        <v>-0.63343400000000005</v>
-      </c>
-      <c r="I28">
-        <v>5.2970199999999998</v>
-      </c>
-      <c r="J28">
-        <v>-3.5557599999999998</v>
-      </c>
-      <c r="K28">
-        <v>-1.4997100000000001</v>
-      </c>
-      <c r="L28">
-        <v>15.5282</v>
-      </c>
-      <c r="M28">
-        <v>-5.9825400000000002</v>
-      </c>
-      <c r="N28">
-        <v>-0.26700400000000002</v>
-      </c>
-      <c r="O28">
-        <v>38.7074</v>
-      </c>
-      <c r="P28">
-        <v>-5.8252899999999999</v>
-      </c>
-      <c r="Q28">
-        <v>0.70436200000000004</v>
-      </c>
-      <c r="R28">
-        <v>51.676600000000001</v>
-      </c>
-      <c r="S28">
-        <v>-1.9110199999999999</v>
-      </c>
-      <c r="T28">
-        <v>-2.0596700000000001</v>
-      </c>
-      <c r="U28">
-        <v>37.764699999999998</v>
-      </c>
-      <c r="V28">
-        <v>2.4549099999999999</v>
-      </c>
-      <c r="W28">
-        <v>-16.447700000000001</v>
-      </c>
-      <c r="X28">
-        <v>38.4572</v>
-      </c>
-      <c r="Y28">
-        <v>-1.7028799999999999</v>
-      </c>
-      <c r="Z28">
-        <v>-23.664200000000001</v>
-      </c>
-      <c r="AA28">
-        <v>11.478999999999999</v>
-      </c>
-      <c r="AB28">
-        <v>-9.8021799999999999</v>
-      </c>
-      <c r="AC28">
-        <v>-25.409800000000001</v>
-      </c>
-      <c r="AD28">
-        <v>-12.0505</v>
-      </c>
-      <c r="AE28">
-        <v>-15.431100000000001</v>
-      </c>
-      <c r="AF28">
-        <v>2.6072299999999999</v>
-      </c>
-      <c r="AG28">
-        <v>37.518799999999999</v>
-      </c>
-      <c r="AH28">
-        <v>2.1113400000000002</v>
-      </c>
-      <c r="AI28">
-        <v>16.252300000000002</v>
-      </c>
-      <c r="AJ28">
-        <v>37.310099999999998</v>
-      </c>
-      <c r="AK28">
-        <v>-4.09117</v>
-      </c>
-      <c r="AL28">
-        <v>21.534800000000001</v>
-      </c>
-      <c r="AM28">
-        <v>12.086600000000001</v>
-      </c>
-      <c r="AN28">
-        <v>9.3762100000000004</v>
-      </c>
-      <c r="AO28">
-        <v>13.2493</v>
-      </c>
-      <c r="AP28">
-        <v>34.797800000000002</v>
-      </c>
-      <c r="AQ28">
-        <v>11.354699999999999</v>
-      </c>
-      <c r="AR28">
-        <v>-8.6593</v>
-      </c>
-      <c r="AS28">
-        <v>-8.8333700000000004</v>
-      </c>
-      <c r="AT28">
-        <v>1.15625</v>
-      </c>
-      <c r="AU28">
-        <v>-8.9584399999999995</v>
-      </c>
-      <c r="AV28">
-        <v>-50.199199999999998</v>
-      </c>
-      <c r="AW28">
-        <v>10.652699999999999</v>
-      </c>
-      <c r="AX28">
-        <v>-9.5631799999999991</v>
-      </c>
-      <c r="AY28">
-        <v>-90.538799999999995</v>
-      </c>
-      <c r="AZ28">
-        <v>0.2276</v>
-      </c>
-      <c r="BA28">
-        <v>10.7005</v>
-      </c>
-      <c r="BB28">
-        <v>-6.8098099999999997</v>
-      </c>
-      <c r="BC28">
-        <v>-0.20275399999999999</v>
-      </c>
-      <c r="BD28">
-        <v>11.0412</v>
-      </c>
-      <c r="BE28">
-        <v>-49.2303</v>
-      </c>
-      <c r="BF28">
-        <v>-1.5501</v>
-      </c>
-      <c r="BG28">
-        <v>7.9818199999999999</v>
-      </c>
-      <c r="BH28">
-        <v>-90.748199999999997</v>
-      </c>
-      <c r="BI28">
-        <v>-3.3494000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>224</v>
-      </c>
-      <c r="B29">
-        <v>1.45038</v>
-      </c>
-      <c r="C29">
-        <v>-11.8682</v>
-      </c>
-      <c r="D29">
-        <v>1.45451</v>
-      </c>
-      <c r="E29">
-        <v>0.203043</v>
-      </c>
-      <c r="F29">
-        <v>-2.9858099999999999</v>
-      </c>
-      <c r="G29">
-        <v>-3.7496499999999999</v>
-      </c>
-      <c r="H29">
-        <v>-0.62502000000000002</v>
-      </c>
-      <c r="I29">
-        <v>5.3053299999999997</v>
-      </c>
-      <c r="J29">
-        <v>-3.5734499999999998</v>
-      </c>
-      <c r="K29">
-        <v>-1.4570099999999999</v>
-      </c>
-      <c r="L29">
-        <v>15.529</v>
-      </c>
-      <c r="M29">
-        <v>-6.0435400000000001</v>
-      </c>
-      <c r="N29">
-        <v>-0.18549499999999999</v>
-      </c>
-      <c r="O29">
-        <v>38.706400000000002</v>
-      </c>
-      <c r="P29">
-        <v>-5.9283200000000003</v>
-      </c>
-      <c r="Q29">
-        <v>0.80286599999999997</v>
-      </c>
-      <c r="R29">
-        <v>51.681199999999997</v>
-      </c>
-      <c r="S29">
-        <v>-2.0372300000000001</v>
-      </c>
-      <c r="T29">
-        <v>-1.98996</v>
-      </c>
-      <c r="U29">
-        <v>37.782200000000003</v>
-      </c>
-      <c r="V29">
-        <v>2.35141</v>
-      </c>
-      <c r="W29">
-        <v>-16.374199999999998</v>
-      </c>
-      <c r="X29">
-        <v>38.426499999999997</v>
-      </c>
-      <c r="Y29">
-        <v>-1.82721</v>
-      </c>
-      <c r="Z29">
-        <v>-23.507400000000001</v>
-      </c>
-      <c r="AA29">
-        <v>11.2149</v>
-      </c>
-      <c r="AB29">
-        <v>-9.1860700000000008</v>
-      </c>
-      <c r="AC29">
-        <v>-25.0839</v>
-      </c>
-      <c r="AD29">
-        <v>-12.420400000000001</v>
-      </c>
-      <c r="AE29">
-        <v>-14.4062</v>
-      </c>
-      <c r="AF29">
-        <v>2.6769400000000001</v>
-      </c>
-      <c r="AG29">
-        <v>37.527900000000002</v>
-      </c>
-      <c r="AH29">
-        <v>2.0140799999999999</v>
-      </c>
-      <c r="AI29">
-        <v>16.3306</v>
-      </c>
-      <c r="AJ29">
-        <v>37.329300000000003</v>
-      </c>
-      <c r="AK29">
-        <v>-4.1699000000000002</v>
-      </c>
-      <c r="AL29">
-        <v>21.843699999999998</v>
-      </c>
-      <c r="AM29">
-        <v>12.3505</v>
-      </c>
-      <c r="AN29">
-        <v>9.6564700000000006</v>
-      </c>
-      <c r="AO29">
-        <v>13.366199999999999</v>
-      </c>
-      <c r="AP29">
-        <v>34.953800000000001</v>
-      </c>
-      <c r="AQ29">
-        <v>12.020300000000001</v>
-      </c>
-      <c r="AR29">
-        <v>-8.7091700000000003</v>
-      </c>
-      <c r="AS29">
-        <v>-8.7806200000000008</v>
-      </c>
-      <c r="AT29">
-        <v>1.1718900000000001</v>
-      </c>
-      <c r="AU29">
-        <v>-9.2447199999999992</v>
-      </c>
-      <c r="AV29">
-        <v>-50.2166</v>
-      </c>
-      <c r="AW29">
-        <v>10.3469</v>
-      </c>
-      <c r="AX29">
-        <v>-9.8329900000000006</v>
-      </c>
-      <c r="AY29">
-        <v>-90.615899999999996</v>
-      </c>
-      <c r="AZ29">
-        <v>0.15495999999999999</v>
-      </c>
-      <c r="BA29">
-        <v>10.6614</v>
-      </c>
-      <c r="BB29">
-        <v>-6.8182299999999998</v>
-      </c>
-      <c r="BC29">
-        <v>-0.121987</v>
-      </c>
-      <c r="BD29">
-        <v>10.972899999999999</v>
-      </c>
-      <c r="BE29">
-        <v>-49.241500000000002</v>
-      </c>
-      <c r="BF29">
-        <v>-1.38683</v>
-      </c>
-      <c r="BG29">
-        <v>8.0592199999999998</v>
-      </c>
-      <c r="BH29">
-        <v>-90.762100000000004</v>
-      </c>
-      <c r="BI29">
-        <v>-3.3579500000000002</v>
-      </c>
-    </row>
     <row r="34" spans="8:58" x14ac:dyDescent="0.2">
       <c r="BF34" s="1"/>
     </row>

</xml_diff>